<commit_message>
uppdate DC to DC converter in the BOM
</commit_message>
<xml_diff>
--- a/docs/Poseidon Bom V1.0 en.xlsx
+++ b/docs/Poseidon Bom V1.0 en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loup_\Documents\Poseidon\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1704B05B-F14C-4FF4-93AD-DDF614BD2DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDF89B6-8F2D-43D6-9C92-80972CAC8C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="2565" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Projet Hydro B</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Digikey</t>
   </si>
   <si>
-    <t>APXW005A0X3-SRZ</t>
-  </si>
-  <si>
-    <t>PDQE10-Q24-S24-D</t>
-  </si>
-  <si>
     <t>GPS</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>BNO-055</t>
   </si>
   <si>
-    <t>Imaginex 852</t>
-  </si>
-  <si>
     <t>Mosaic X5 / Piksi / Zed-F9P</t>
   </si>
   <si>
@@ -118,6 +109,24 @@
   </si>
   <si>
     <t xml:space="preserve">*1 The USB connector may vary from one gps module to another. </t>
+  </si>
+  <si>
+    <t>PYBE20-Q24-S5-T</t>
+  </si>
+  <si>
+    <t>PYBE20-Q24-S24-T</t>
+  </si>
+  <si>
+    <t>Only for the Sonar *2</t>
+  </si>
+  <si>
+    <t>*2 you can verify with Imagenex if your sonar is comptatible with 12v supply</t>
+  </si>
+  <si>
+    <t>if yes you can ommit the 24v suply</t>
+  </si>
+  <si>
+    <t>Imagenex 852</t>
   </si>
 </sst>
 </file>
@@ -469,7 +478,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -510,10 +519,10 @@
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -522,10 +531,10 @@
     </row>
     <row r="5" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
@@ -533,10 +542,10 @@
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -545,18 +554,18 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -567,10 +576,10 @@
     </row>
     <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -579,13 +588,16 @@
     </row>
     <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="E11" s="6"/>
     </row>
@@ -598,13 +610,13 @@
     </row>
     <row r="13" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B13" s="7">
         <v>15817</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -612,24 +624,24 @@
     </row>
     <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
@@ -639,17 +651,17 @@
     </row>
     <row r="18" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="9"/>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E19" s="11"/>
     </row>
@@ -666,7 +678,7 @@
     </row>
     <row r="22" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" s="4"/>
       <c r="E22" s="11"/>
@@ -677,12 +689,18 @@
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="B24" s="4"/>
       <c r="D24" s="10"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="26" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>